<commit_message>
finished results for day 0 and day 107
</commit_message>
<xml_diff>
--- a/output/GlucoseEffectDay0_Day107Results.xlsx
+++ b/output/GlucoseEffectDay0_Day107Results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usu-my.sharepoint.com/personal/a02308724_aggies_usu_edu/Documents/Desktop/ASU green iguana 2021/greeniguanaAnalysis/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A95B6748-5AD2-4C6E-9AE8-1E295F5B3759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="117" documentId="8_{A95B6748-5AD2-4C6E-9AE8-1E295F5B3759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BEAAE9EC-ADEB-41C7-A6FA-F50F51912495}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0AEC4978-5AE5-4C01-8C64-F391ED922A9D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="82">
   <si>
     <t>Dependent Variable</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Statistical results of a one way ANOVA on the effect of glucose across entire experiment comparing initial and final time point.</t>
   </si>
   <si>
-    <t>TukeyHSD</t>
-  </si>
-  <si>
     <t>Both groups on day 107 are higher than groups on day 0. Groups not different on day 0. Glucose group higher than water group on day 107.</t>
   </si>
   <si>
@@ -155,6 +152,135 @@
   </si>
   <si>
     <t>64.7 ± 3.4, 18</t>
+  </si>
+  <si>
+    <t>kruskal</t>
+  </si>
+  <si>
+    <t>chi sq is 49.26</t>
+  </si>
+  <si>
+    <t>0.094 ± 0.04, 17</t>
+  </si>
+  <si>
+    <t>3.43 ± 0.635, 17</t>
+  </si>
+  <si>
+    <t>0.041 ± 0.021, 16</t>
+  </si>
+  <si>
+    <t>0.939 ± 0.167, 18</t>
+  </si>
+  <si>
+    <t>tukey or wilcoxin</t>
+  </si>
+  <si>
+    <t>chi sq is 41.623</t>
+  </si>
+  <si>
+    <t>Glucose on day 107 is higher than glucose on day 0 but same as water on day 0. Water on day 107 is higher than glucose day 0 and water day 0. within groups is not different on either day.</t>
+  </si>
+  <si>
+    <t>Both groups on day 107 are higher than groups on day 0. within groups not different on day 0 and day 107.</t>
+  </si>
+  <si>
+    <t>chisq is 7.424</t>
+  </si>
+  <si>
+    <t>post hoc not sig but based on ggplot, day 107sugar different from all other groups</t>
+  </si>
+  <si>
+    <t>chi sq is 4.772</t>
+  </si>
+  <si>
+    <t>chi sq is 8.249</t>
+  </si>
+  <si>
+    <t>Nothing siginficant, the only thing close to significance is between water 0 and glucose 0 at 0.084</t>
+  </si>
+  <si>
+    <t>2.35 ± 0.329,18</t>
+  </si>
+  <si>
+    <t>3.64 ± 0.981, 14</t>
+  </si>
+  <si>
+    <t>1.19 ± 0.267, 16</t>
+  </si>
+  <si>
+    <t>2.28 ± 0.343,18</t>
+  </si>
+  <si>
+    <t>216 ± 11.9, 18</t>
+  </si>
+  <si>
+    <t>303 ± 16, 18</t>
+  </si>
+  <si>
+    <t>259 ± 11.2, 18</t>
+  </si>
+  <si>
+    <t>324 ± 14.5, 18</t>
+  </si>
+  <si>
+    <t>0.243 ± 0.265, 18</t>
+  </si>
+  <si>
+    <t>-0.024 ± 0.208, 17</t>
+  </si>
+  <si>
+    <t>-0.243 ± 0.193, 18</t>
+  </si>
+  <si>
+    <t>0.022 ± 0.27, 18</t>
+  </si>
+  <si>
+    <t>-0.026 ± 0.272, 18</t>
+  </si>
+  <si>
+    <t>-0.421 ± 0.166, 18</t>
+  </si>
+  <si>
+    <t>0.026 ± 0.201, 18</t>
+  </si>
+  <si>
+    <t>0.319 ± 0.279, 18</t>
+  </si>
+  <si>
+    <t>-0.269 ± 0.389, 18</t>
+  </si>
+  <si>
+    <t>-0.314 ± 0.272, 17</t>
+  </si>
+  <si>
+    <t>0.269 ± 0.323, 18</t>
+  </si>
+  <si>
+    <t>0.297 ± 0.455, 18</t>
+  </si>
+  <si>
+    <t>2.68 ± 0.381, 18</t>
+  </si>
+  <si>
+    <t>3.14 ± 0.922, 14</t>
+  </si>
+  <si>
+    <t>1.90 ± 0.369, 16</t>
+  </si>
+  <si>
+    <t>1.56 ± 0.308, 18</t>
+  </si>
+  <si>
+    <t>80.2 ± 6.04, 18</t>
+  </si>
+  <si>
+    <t>50.2 ± 9.0, 18</t>
+  </si>
+  <si>
+    <t>76.5 ± 7.51, 18</t>
+  </si>
+  <si>
+    <t>84.9 ± 2.80, 18</t>
   </si>
 </sst>
 </file>
@@ -333,12 +459,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -346,16 +468,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -373,7 +491,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,28 +812,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C421DD5-04DE-400C-98C2-B6FB818C73BD}">
-  <dimension ref="B3:O36"/>
+  <dimension ref="A3:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" customWidth="1"/>
+    <col min="4" max="4" width="17.90625" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" customWidth="1"/>
+    <col min="6" max="6" width="159.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.453125" customWidth="1"/>
+    <col min="8" max="8" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.81640625" customWidth="1"/>
+    <col min="11" max="11" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>27</v>
       </c>
@@ -717,344 +842,479 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="25" t="s">
+    <row r="4" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="22">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="11">
+        <v>63.89</v>
+      </c>
+      <c r="D6" s="22">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="28" t="s">
+    <row r="7" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="22">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B8" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="11">
+        <v>12.71</v>
+      </c>
+      <c r="D8" s="22">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="D9" s="22">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="F9" s="25"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B10" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="11">
+        <v>1.6830000000000001</v>
+      </c>
+      <c r="D10" s="22">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="F10" s="25"/>
+    </row>
+    <row r="11" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B11" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="11">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="D11" s="22">
+        <v>3</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="F11" s="25"/>
+    </row>
+    <row r="12" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="22">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="O12" s="15"/>
+    </row>
+    <row r="13" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="22">
+        <v>3</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.189</v>
+      </c>
+      <c r="F13" s="25"/>
+      <c r="O13" s="14"/>
+    </row>
+    <row r="14" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="22">
+        <v>3</v>
+      </c>
+      <c r="E14" s="3">
+        <v>4.1099999999999998E-2</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="O14" s="14"/>
+    </row>
+    <row r="15" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B15" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="4">
+        <v>9.1389999999999993</v>
+      </c>
+      <c r="D15" s="24">
+        <v>3</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="O15" s="14"/>
+    </row>
+    <row r="16" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B16" s="14"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="O16" s="14"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="O17" s="14"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B19" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="16">
-        <v>30.74</v>
-      </c>
-      <c r="D5" s="28">
-        <v>3</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="28" t="s">
+      <c r="C19" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B20" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="28" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="16">
-        <v>63.89</v>
-      </c>
-      <c r="D6" s="28">
-        <v>3</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="28" t="s">
+      <c r="D20" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B21" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="28">
-        <v>3</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="31"/>
-    </row>
-    <row r="8" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="28">
-        <v>3</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="31"/>
-    </row>
-    <row r="9" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="28" t="s">
+      <c r="C21" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B22" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B23" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="28">
-        <v>3</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="31"/>
-    </row>
-    <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="28" t="s">
+      <c r="C23" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B24" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="28">
-        <v>3</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="31"/>
-    </row>
-    <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="28" t="s">
+      <c r="C24" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" s="31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B25" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="28">
-        <v>3</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="31"/>
-    </row>
-    <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="28" t="s">
+      <c r="C25" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B26" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="28">
-        <v>3</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="31"/>
-      <c r="O12" s="20"/>
-    </row>
-    <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="28">
-        <v>3</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="31"/>
-      <c r="O13" s="19"/>
-    </row>
-    <row r="14" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="28">
-        <v>3</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="31"/>
-      <c r="O14" s="19"/>
-    </row>
-    <row r="15" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="5">
-        <v>9.1389999999999993</v>
-      </c>
-      <c r="D15" s="30">
-        <v>3</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="32" t="s">
+      <c r="C26" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="F26" s="31" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B27" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B28" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B29" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="O15" s="19"/>
-    </row>
-    <row r="16" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="O16" s="19"/>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="O17" s="19"/>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="19"/>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="19"/>
-      <c r="F22" s="12"/>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="19"/>
-      <c r="F23" s="12"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="19"/>
-      <c r="F24" s="12"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="19"/>
-      <c r="F25" s="12"/>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="19"/>
-      <c r="F26" s="12"/>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="19"/>
-      <c r="F27" s="12"/>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="19"/>
-      <c r="F28" s="12"/>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="14" t="s">
+      <c r="D29" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="E29" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="F29" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F29" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="23"/>
-    </row>
-    <row r="31" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="22"/>
-    </row>
-    <row r="32" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="23"/>
-    </row>
-    <row r="33" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="24"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
+    </row>
+    <row r="30" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="17"/>
+    </row>
+    <row r="31" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="16"/>
+    </row>
+    <row r="32" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="17"/>
+    </row>
+    <row r="33" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="18"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>